<commit_message>
Seychelles updated ; Named build arguments
</commit_message>
<xml_diff>
--- a/wildlife/reports/Seychelles/composition/Port Launay/Birds/composition.xlsx
+++ b/wildlife/reports/Seychelles/composition/Port Launay/Birds/composition.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -532,6 +532,16 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Striated Heron</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>